<commit_message>
iter 3 sampling complete
</commit_message>
<xml_diff>
--- a/data/final_data/bests_models_results.xlsx
+++ b/data/final_data/bests_models_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,11 +464,6 @@
           <t>r2</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Tiempo de Ejecución</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -478,7 +473,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>iter2-cov</t>
+          <t>iter3-UnderSampling</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -497,16 +492,13 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.8376728270197041</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2.591475963592529</v>
+        <v>0.8469430984397408</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>new_values</t>
+          <t>new_values_log</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -516,90 +508,81 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>FL</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Lasso</t>
+          <t>RandomForest</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>{'model__alpha': 1.0}</t>
+          <t>{'model__n_estimators': 50}</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.8788511235177607</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.1335110664367676</v>
+        <v>0.8376728270197041</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>new_values</t>
+          <t>new_values_log</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>iter2-cov</t>
+          <t>iter3-OverSampling</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>FL</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>LinearRegression</t>
+          <t>RandomForest</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>{'model__n_estimators': 50}</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.9119573949198786</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.02905392646789551</v>
+        <v>0.8358860457707065</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>all_log</t>
+          <t>new_values</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>iter2-cov</t>
+          <t>iter3-OverSampling</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>GA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>AdaBoost</t>
+          <t>Lasso</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>{'model__n_estimators': 50}</t>
+          <t>{'model__alpha': 1.0}</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.6143037383604859</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1.878231048583984</v>
+        <v>0.9001475754583788</v>
       </c>
     </row>
     <row r="6">
@@ -610,29 +593,26 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>iter1-normal</t>
+          <t>iter3-UnderSampling</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>GA</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>GradientBoosting</t>
+          <t>Lasso</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>{'model__n_estimators': 150}</t>
+          <t>{'model__alpha': 1.0}</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.9060651223899857</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.4907262325286865</v>
+        <v>0.9001258546622485</v>
       </c>
     </row>
     <row r="7">
@@ -648,7 +628,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>GA</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -662,10 +642,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.8355560181287938</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.1041080951690674</v>
+        <v>0.8788511235177607</v>
       </c>
     </row>
     <row r="8">
@@ -676,29 +653,446 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>iter3-OverSampling</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>LinearRegression</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.9176460433793464</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>new_values</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>iter3-UnderSampling</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>LinearRegression</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0.9176460433793464</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>new_values</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>iter2-cov</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>LinearRegression</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0.9119573949198786</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>all_log</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>iter3-OverSampling</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NJ</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>AdaBoost</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>{'model__n_estimators': 50}</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0.9017978960530233</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>all_log</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>iter3-UnderSampling</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NJ</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>AdaBoost</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>{'model__n_estimators': 50}</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>0.7997092373207666</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>all_log</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>iter2-cov</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NJ</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>AdaBoost</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>{'model__n_estimators': 50}</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>0.6143037383604859</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>new_values</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>iter3-UnderSampling</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NY</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>GradientBoosting</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>{'model__n_estimators': 150}</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0.9529815385623106</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>new_values</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>iter3-OverSampling</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NY</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>GradientBoosting</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>{'model__n_estimators': 150}</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>0.9403092362887392</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>new_values</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>iter1-normal</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NY</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>GradientBoosting</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>{'model__n_estimators': 150}</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>0.9060651223899857</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>new_values</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>iter3-OverSampling</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Lasso</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>{'model__alpha': 1.0}</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>0.8458742226569919</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>new_values</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>iter3-UnderSampling</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Lasso</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>{'model__alpha': 1.0}</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>0.8458742226569919</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>new_values</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>iter2-cov</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Lasso</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>{'model__alpha': 1.0}</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>0.8355560181287938</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>new_values</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>iter3-OverSampling</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
         <is>
           <t>VA</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>LinearRegression</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>{}</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="F20" t="n">
+        <v>0.9409347961886814</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>new_values</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>iter3-UnderSampling</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>LinearRegression</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>0.9409347961886814</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>new_values</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>iter2-cov</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>LinearRegression</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
         <v>0.9211187366768711</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.02756190299987793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>